<commit_message>
Add the auto increment for ID
</commit_message>
<xml_diff>
--- a/src/main/resources/DB.xlsx
+++ b/src/main/resources/DB.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2715" windowWidth="22050" windowHeight="6315"/>
@@ -9,17 +9,14 @@
   <sheets>
     <sheet name="DB" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="48">
   <si>
     <t>Rex</t>
-  </si>
-  <si>
-    <t>NOT NULL PRIMARY KEY</t>
   </si>
   <si>
     <t>INPUT_DATE</t>
@@ -161,17 +158,23 @@
   </si>
   <si>
     <t>ROLE_NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOT NULL PRIMARY KEY auto_increment </t>
+  </si>
+  <si>
+    <t>int(8)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -179,13 +182,13 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -245,27 +248,98 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="C7EDCC"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -300,7 +374,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -335,7 +409,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -546,47 +620,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="H53" sqref="H53"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51:E58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="46.875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.125" style="3"/>
+    <col min="3" max="3" width="37.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" ht="18.75">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="2">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1" s="4">
         <v>42145</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" ht="18.75">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" ht="18.75">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>0</v>
@@ -598,46 +672,46 @@
         <v>drop table BDM_USER_T;</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="18.75" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" ht="18.75">
       <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="E4" s="3" t="str">
         <f>"create table "&amp;B2&amp;" ("</f>
         <v>create table BDM_USER_T (</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="3" t="str">
         <f>A5&amp;" "&amp;B5&amp;" "&amp;C5&amp;", "</f>
-        <v xml:space="preserve">ID DECIMAL(10,0) NOT NULL PRIMARY KEY, </v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+        <v xml:space="preserve">ID int(8) NOT NULL PRIMARY KEY auto_increment , </v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -646,12 +720,12 @@
         <v xml:space="preserve">LOGIN_NAME VARCHAR(100) , </v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -660,12 +734,12 @@
         <v xml:space="preserve">LOGIN_PASSWORD VARCHAR(100) , </v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -674,12 +748,12 @@
         <v xml:space="preserve">USER_NAME VARCHAR(100) , </v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5">
       <c r="A9" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -688,60 +762,60 @@
         <v xml:space="preserve">TOKEN VARCHAR(100) , </v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5">
       <c r="A10" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E10" s="3" t="str">
         <f t="shared" ref="E10:E17" si="1">A10&amp;" "&amp;B10&amp;" "&amp;C10&amp;", "</f>
         <v xml:space="preserve">ROLE VARCHAR(2) , </v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E11" s="3" t="str">
         <f t="shared" ref="E11" si="2">A11&amp;" "&amp;B11&amp;" "&amp;C11&amp;", "</f>
         <v xml:space="preserve">STATUS VARCHAR(2) , </v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E12" s="3" t="str">
         <f t="shared" ref="E12:E16" si="3">A12&amp;" "&amp;B12&amp;" "&amp;C12&amp;", "</f>
         <v xml:space="preserve">MARKER_FLAG VARCHAR(2) , </v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="5"/>
@@ -750,12 +824,12 @@
         <v xml:space="preserve">INPUT_NAME VARCHAR(100) , </v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5">
       <c r="A14" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="5"/>
@@ -764,12 +838,12 @@
         <v xml:space="preserve">INPUT_DATE VARCHAR(100) , </v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5">
       <c r="A15" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="5"/>
@@ -778,12 +852,12 @@
         <v xml:space="preserve">UPDATE_NAME VARCHAR(100) , </v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5">
       <c r="A16" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="5"/>
@@ -792,49 +866,49 @@
         <v xml:space="preserve">UPDATE_DATE VARCHAR(100) , </v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5">
       <c r="A17" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E17" s="3" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">DELSIGN DECIMAL(1,0) , </v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="18.75" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" ht="18.75">
       <c r="A19" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B19" s="2">
         <v>2</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D19" s="4">
         <v>42145</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="18.75" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" ht="18.75">
       <c r="A20" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:5" ht="18.75" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" ht="18.75">
       <c r="A21" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>0</v>
@@ -846,46 +920,46 @@
         <v>drop table BDM_MARKER_T;</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="18.75" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" ht="18.75">
       <c r="A22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="E22" s="3" t="str">
         <f>"create table "&amp;B20&amp;" ("</f>
         <v>create table BDM_MARKER_T (</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5">
       <c r="A23" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="3" t="str">
         <f>A23&amp;" "&amp;B23&amp;" "&amp;C23&amp;", "</f>
-        <v xml:space="preserve">MARKER_ID DECIMAL(10,0) NOT NULL PRIMARY KEY, </v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+        <v xml:space="preserve">MARKER_ID int(8) NOT NULL PRIMARY KEY auto_increment , </v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -894,12 +968,12 @@
         <v xml:space="preserve">MARKER_NAME VARCHAR(500) , </v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5">
       <c r="A25" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -908,44 +982,44 @@
         <v xml:space="preserve">MARKER_TYPE VARCHAR(500) , </v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5">
       <c r="A26" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E26" s="3" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve">MARKER_LNGLAT VARCHAR(100) , </v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5">
       <c r="A27" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E27" s="3" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve">MARKER_ADDRESS VARCHAR(500) , </v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5">
       <c r="A28" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="5"/>
@@ -954,12 +1028,12 @@
         <v xml:space="preserve">INPUT_NAME VARCHAR(100) , </v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5">
       <c r="A29" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="5"/>
@@ -968,12 +1042,12 @@
         <v xml:space="preserve">INPUT_DATE VARCHAR(100) , </v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5">
       <c r="A30" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="5"/>
@@ -982,12 +1056,12 @@
         <v xml:space="preserve">UPDATE_NAME VARCHAR(100) , </v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5">
       <c r="A31" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="5"/>
@@ -996,49 +1070,49 @@
         <v xml:space="preserve">UPDATE_DATE VARCHAR(100) , </v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5">
       <c r="A32" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E32" s="3" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve">DELSIGN DECIMAL(1,0) , </v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="18.75" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:5" ht="18.75">
       <c r="A34" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B34" s="2">
         <v>3</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D34" s="4">
         <v>42145</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="18.75" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:5" ht="18.75">
       <c r="A35" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="1:5" ht="18.75" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:5" ht="18.75">
       <c r="A36" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>0</v>
@@ -1050,46 +1124,46 @@
         <v>drop table BDM_TYPE_T;</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="18.75" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:5" ht="18.75">
       <c r="A37" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="C37" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="D37" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="E37" s="3" t="str">
         <f>"create table "&amp;B35&amp;" ("</f>
         <v>create table BDM_TYPE_T (</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:5">
       <c r="A38" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="3" t="str">
         <f>A38&amp;" "&amp;B38&amp;" "&amp;C38&amp;", "</f>
-        <v xml:space="preserve">TYPE_ID DECIMAL(10,0) NOT NULL PRIMARY KEY, </v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
+        <v xml:space="preserve">TYPE_ID int(8) NOT NULL PRIMARY KEY auto_increment , </v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -1098,12 +1172,12 @@
         <v xml:space="preserve">TYPE_NAME VARCHAR(500) , </v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:5">
       <c r="A40" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -1112,12 +1186,12 @@
         <v xml:space="preserve">TYPE_LEVEL VARCHAR(500) , </v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:5">
       <c r="A41" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -1126,12 +1200,12 @@
         <v xml:space="preserve">TYPE_PARENT_ID DECIMAL(10,0) , </v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:5">
       <c r="A42" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="5"/>
@@ -1140,12 +1214,12 @@
         <v xml:space="preserve">INPUT_NAME VARCHAR(100) , </v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:5">
       <c r="A43" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="5"/>
@@ -1154,12 +1228,12 @@
         <v xml:space="preserve">INPUT_DATE VARCHAR(100) , </v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:5">
       <c r="A44" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="5"/>
@@ -1168,12 +1242,12 @@
         <v xml:space="preserve">UPDATE_NAME VARCHAR(100) , </v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:5">
       <c r="A45" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="5"/>
@@ -1182,49 +1256,49 @@
         <v xml:space="preserve">UPDATE_DATE VARCHAR(100) , </v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:5">
       <c r="A46" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E46" s="3" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">DELSIGN DECIMAL(1,0) , </v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="18.75" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:5" ht="18.75">
       <c r="A48" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B48" s="2">
         <v>4</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D48" s="4">
         <v>42165</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="18.75" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:5" ht="18.75">
       <c r="A49" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
     </row>
-    <row r="50" spans="1:5" ht="18.75" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:5" ht="18.75">
       <c r="A50" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>0</v>
@@ -1236,46 +1310,46 @@
         <v>drop table BDM_ROLE_T;</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="18.75" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:5" ht="18.75">
       <c r="A51" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="D51" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="E51" s="3" t="str">
         <f>"create table "&amp;B49&amp;" ("</f>
         <v>create table BDM_ROLE_T (</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:5">
       <c r="A52" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="3" t="str">
         <f>A52&amp;" "&amp;B52&amp;" "&amp;C52&amp;", "</f>
-        <v xml:space="preserve">ROLE_ID DECIMAL(10,0) NOT NULL PRIMARY KEY, </v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.15">
+        <v xml:space="preserve">ROLE_ID int(8) NOT NULL PRIMARY KEY auto_increment , </v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
       <c r="A53" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
@@ -1284,12 +1358,12 @@
         <v xml:space="preserve">ROLE_NAME VARCHAR(500) , </v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:5">
       <c r="A54" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="5"/>
@@ -1298,12 +1372,12 @@
         <v xml:space="preserve">INPUT_NAME VARCHAR(100) , </v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:5">
       <c r="A55" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="5"/>
@@ -1312,12 +1386,12 @@
         <v xml:space="preserve">INPUT_DATE VARCHAR(100) , </v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:5">
       <c r="A56" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="5"/>
@@ -1326,12 +1400,12 @@
         <v xml:space="preserve">UPDATE_NAME VARCHAR(100) , </v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:5">
       <c r="A57" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="5"/>
@@ -1340,149 +1414,149 @@
         <v xml:space="preserve">UPDATE_DATE VARCHAR(100) , </v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:5">
       <c r="A58" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E58" s="3" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve">DELSIGN DECIMAL(1,0) , </v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="18.75" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:5" ht="18.75">
       <c r="A60" s="1"/>
       <c r="B60" s="2"/>
       <c r="C60" s="1"/>
       <c r="D60" s="4"/>
     </row>
-    <row r="61" spans="1:5" ht="18.75" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:5" ht="18.75">
       <c r="A61" s="1"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
     </row>
-    <row r="62" spans="1:5" ht="18.75" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:5" ht="18.75">
       <c r="A62" s="1"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
     </row>
-    <row r="63" spans="1:5" ht="18.75" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:5" ht="18.75">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:5">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:4">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:4">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="5"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:4">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="5"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:4">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="5"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:4">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="5"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:4">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
     </row>
-    <row r="72" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:4" ht="18.75">
       <c r="A72" s="1"/>
       <c r="B72" s="2"/>
       <c r="C72" s="1"/>
       <c r="D72" s="4"/>
     </row>
-    <row r="73" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:4" ht="18.75">
       <c r="A73" s="1"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
     </row>
-    <row r="74" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:4" ht="18.75">
       <c r="A74" s="1"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
     </row>
-    <row r="75" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:4" ht="18.75">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:4">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:4">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:4">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
       <c r="D78" s="5"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:4">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
       <c r="D79" s="5"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:4">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
       <c r="D80" s="5"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:4">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
       <c r="D81" s="5"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:4">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>

</xml_diff>